<commit_message>
added chord notes finder in webapp
</commit_message>
<xml_diff>
--- a/datasets/allScalesAndFormulae.xlsx
+++ b/datasets/allScalesAndFormulae.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\SomethingExtra\Project_Chord_Scale_python\MusicMakingGuide\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932AF89A-DCCE-42D2-A53F-E619190A7E7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1FA93D-2B51-496B-B48B-361E767D1675}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>